<commit_message>
add kCar to PlotShearFlow
</commit_message>
<xml_diff>
--- a/custom plots/10pct_0WSt_and_iCar-Thixotropy_031024_fit.xlsx
+++ b/custom plots/10pct_0WSt_and_iCar-Thixotropy_031024_fit.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,6 +595,81 @@
         <v>3.442918254066386</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>10%_0WSt_kCar_1</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-164.5681764470073</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3.645852121809451</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.07752968282954108</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.002211246080797293</v>
+      </c>
+      <c r="F7" t="n">
+        <v>404.0117296072254</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3.491151435698671</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>10%_0WSt_kCar_2</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-130.5920206515675</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3.223792544422935</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.08099504891644603</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.002479759855658115</v>
+      </c>
+      <c r="F8" t="n">
+        <v>390.4951195188706</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3.098563056362585</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>10%_0WSt_kCar_3</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-62.0559463280163</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2.988344031710459</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.1922832153837944</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.006000398964713743</v>
+      </c>
+      <c r="F9" t="n">
+        <v>541.0181235241719</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3.373781092379696</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>